<commit_message>
Set VMP BNF codes when we think they can be inferred
</commit_message>
<xml_diff>
--- a/openprescribing/dmd2/tests/fixtures/bnf_code_mapping/mapping.xlsx
+++ b/openprescribing/dmd2/tests/fixtures/bnf_code_mapping/mapping.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -393,7 +393,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -403,22 +403,27 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>'1003020U0AAAIAI</t>
+          <t>'0203020C0AAAAAA</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Diclofenac Sod_Gel 2.32%</t>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>'22480211000001104</t>
+          <t>'4744111000001109</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% gel</t>
+          <t>Adenosine 6mg/2ml solution for injection vials</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection 6 vials</t>
         </is>
       </c>
     </row>
@@ -435,64 +440,59 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>'1003020U0AAAIAI</t>
+          <t>'0203020C0AAAAAA</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Diclofenac Sod_Gel 2.32%</t>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>'22479411000001100</t>
+          <t>'34516311000001106</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% gel</t>
+          <t>Adenosine 6mg/2ml solution for injection vials</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% 50 grams</t>
+          <t>Adenosine 6mg/2ml solution for injection 5 vials</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMP</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>'1003020U0AAAIAI</t>
+          <t>'0203020C0BBAAAA</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Diclofenac Sod_Gel 2.32%</t>
+          <t>Adenocor_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>'22479511000001101</t>
+          <t>'4744411000001104</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% gel</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Diclofenac 2.32% 30 grams</t>
+          <t>Adenocor 6mg/2ml solution for injection vials (Sanofi)</t>
         </is>
       </c>
     </row>
@@ -504,32 +504,32 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMP</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>'1003020U0AAAIAI</t>
+          <t>'0203020C0BBAAAA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Diclofenac Sod_Gel 2.32%</t>
+          <t>Adenocor_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>'26352411000001101</t>
+          <t>'4744711000001105</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% gel</t>
+          <t>Adenocor 6mg/2ml solution for injection vials (Sanofi)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% 100 grams</t>
+          <t>Adenocor 6mg/2ml solution for injection (Sanofi) 6 vials</t>
         </is>
       </c>
     </row>
@@ -546,22 +546,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>'1003020U0BBADAI</t>
+          <t>'0203020C0AAAAAA</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>'22479611000001102</t>
+          <t>'19663311000001109</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Wockhardt UK Ltd)</t>
         </is>
       </c>
     </row>
@@ -578,34 +578,34 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>'1003020U0BBADAI</t>
+          <t>'0203020C0AAAAAA</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>'22479711000001106</t>
+          <t>'19663411000001102</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Wockhardt UK Ltd)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 50 grams</t>
+          <t>Adenosine 6mg/2ml solution for injection (Wockhardt UK Ltd) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -615,27 +615,22 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>'1003020U0BBADAI</t>
+          <t>'0203020C0AAAAAA</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>'22479911000001108</t>
+          <t>'20009311000001102</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 30 grams</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (A A H Pharmaceuticals Ltd)</t>
         </is>
       </c>
     </row>
@@ -652,27 +647,27 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>'1003020U0BBADAI</t>
+          <t>'0203020C0AAAAAA</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>'26352611000001103</t>
+          <t>'20009411000001109</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (A A H Pharmaceuticals Ltd)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 100 grams</t>
+          <t>Adenosine 6mg/2ml solution for injection (A A H Pharmaceuticals Ltd) 6 vials</t>
         </is>
       </c>
     </row>
@@ -684,17 +679,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>'0203020C0AAAAAA</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>'35084911000001108</t>
+          <t>'21855411000001109</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Tobramycin 200mg/5ml oral solution</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Focus Pharmaceuticals Ltd)</t>
         </is>
       </c>
     </row>
@@ -706,56 +711,71 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>'0203020C0AAAAAA</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>'35085111000001109</t>
+          <t>'21855511000001108</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Tobramycin 200mg/5ml oral solution</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Focus Pharmaceuticals Ltd)</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Tobramycin 200mg/5ml oral 1 ml</t>
+          <t>Adenosine 6mg/2ml solution for injection (Focus Pharmaceuticals Ltd) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>'0203020C0AAAAAA</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>'35085211000001103</t>
+          <t>'24530711000001102</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Tobramycin 200mg/5ml oral solution</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Tobramycin 200mg/5ml oral 30 mls</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Alliance Healthcare (Distribution) Ltd)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -763,21 +783,36 @@
           <t>AMP</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>'0203020C0AAAAAA</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>'35423111000001105</t>
+          <t>'24531011000001108</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Tobramycin 200mg/5ml oral solution (Special Order)</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Alliance Healthcare (Distribution) Ltd)</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection (Alliance Healthcare (Distribution) Ltd) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -785,19 +820,24 @@
           <t>AMP</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>'0203020C0AAAAAA</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>'35423311000001107</t>
+          <t>'34516211000001103</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Tobramycin 200mg/5ml oral solution (Special Order)</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Tobramycin 200mg/5ml oral (Special Order) 1 ml</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Peckforton Pharmaceuticals Ltd)</t>
         </is>
       </c>
     </row>
@@ -812,19 +852,315 @@
           <t>AMP</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>'0203020C0AAAAAA</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+        </is>
+      </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>'35423511000001101</t>
+          <t>'34516411000001104</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Tobramycin 200mg/5ml oral solution (Special Order)</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Peckforton Pharmaceuticals Ltd)</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Tobramycin 200mg/5ml oral (Special Order) 30 mls</t>
+          <t>Adenosine 6mg/2ml solution for injection (Peckforton Pharmaceuticals Ltd) 5 vials</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>'1003020U0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Diclofenac Sod_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>'22480211000001104</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% gel</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>'1003020U0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Diclofenac Sod_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>'22479411000001100</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% gel</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% 50 grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>'1003020U0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Diclofenac Sod_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>'22479511000001101</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% gel</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% 30 grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>'1003020U0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Diclofenac Sod_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>'26352411000001101</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% gel</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% 100 grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>'1003020U0BBADAI</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>'22479611000001102</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>'1003020U0BBADAI</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>'22479711000001106</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 50 grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>'1003020U0BBADAI</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>'22479911000001108</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 30 grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>'1003020U0BBADAI</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>'26352611000001103</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 100 grams</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Set Presentation.dmd_name in import_dmd2
</commit_message>
<xml_diff>
--- a/openprescribing/dmd2/tests/fixtures/bnf_code_mapping/mapping.xlsx
+++ b/openprescribing/dmd2/tests/fixtures/bnf_code_mapping/mapping.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -393,7 +393,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -401,29 +401,14 @@
           <t>VMP</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>'0203020C0AAAAAA</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>'4744111000001109</t>
+          <t>'3549611000001100</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Adenosine 6mg/2ml solution for injection 6 vials</t>
+          <t>Generic Nutrison liquid</t>
         </is>
       </c>
     </row>
@@ -438,61 +423,46 @@
           <t>VMP</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>'0203020C0AAAAAA</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>'34516311000001106</t>
+          <t>'1051411000001107</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials</t>
+          <t>Generic Nutrison liquid</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection 5 vials</t>
+          <t>Generic Nutrison 500 mls</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>AMP</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>'0203020C0BBAAAA</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Adenocor_I/V Inf 3mg/ml 2ml Vl</t>
+          <t>VMP</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>'4744411000001104</t>
+          <t>'998911000001109</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Adenocor 6mg/2ml solution for injection vials (Sanofi)</t>
+          <t>Generic Nutrison liquid</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Generic Nutrison 1000 mls</t>
         </is>
       </c>
     </row>
@@ -504,32 +474,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AMP</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>'0203020C0BBAAAA</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Adenocor_I/V Inf 3mg/ml 2ml Vl</t>
+          <t>VMP</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>'4744711000001105</t>
+          <t>'1045511000001107</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Adenocor 6mg/2ml solution for injection vials (Sanofi)</t>
+          <t>Generic Nutrison liquid</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Adenocor 6mg/2ml solution for injection (Sanofi) 6 vials</t>
+          <t>Generic Nutrison 1500 mls</t>
         </is>
       </c>
     </row>
@@ -546,22 +506,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>'0203020C0AAAAAA</t>
+          <t>'090402000BBDUA0</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+          <t>Nutrison_Liq</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>'19663311000001109</t>
+          <t>'442611000001109</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (Wockhardt UK Ltd)</t>
+          <t>Nutrison liquid (Nutricia Ltd)</t>
         </is>
       </c>
     </row>
@@ -578,34 +538,34 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>'0203020C0AAAAAA</t>
+          <t>'090402000BBDUA0</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+          <t>Nutrison_Liq</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>'19663411000001102</t>
+          <t>'1714711000001106</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (Wockhardt UK Ltd)</t>
+          <t>Nutrison liquid (Nutricia Ltd)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection (Wockhardt UK Ltd) 6 vials</t>
+          <t>Nutrison (Nutricia Ltd) 500 mls</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -615,22 +575,27 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>'0203020C0AAAAAA</t>
+          <t>'090402000BBHCA0</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+          <t>Nutrison Pack_Stnd</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>'20009311000001102</t>
+          <t>'1714811000001103</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (A A H Pharmaceuticals Ltd)</t>
+          <t>Nutrison liquid (Nutricia Ltd)</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Nutrison (Nutricia Ltd) 500 mls</t>
         </is>
       </c>
     </row>
@@ -647,34 +612,34 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>'0203020C0AAAAAA</t>
+          <t>'090402000BBHCA0</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+          <t>Nutrison Pack_Stnd</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>'20009411000001109</t>
+          <t>'1714911000001108</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (A A H Pharmaceuticals Ltd)</t>
+          <t>Nutrison liquid (Nutricia Ltd)</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection (A A H Pharmaceuticals Ltd) 6 vials</t>
+          <t>Nutrison (Nutricia Ltd) 1000 mls</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -684,29 +649,34 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>'0203020C0AAAAAA</t>
+          <t>'090402000BBHCA0</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+          <t>Nutrison Pack_Stnd</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>'21855411000001109</t>
+          <t>'1715011000001108</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (Focus Pharmaceuticals Ltd)</t>
+          <t>Nutrison liquid (Nutricia Ltd)</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Nutrison (Nutricia Ltd) 1500 mls</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -714,36 +684,21 @@
           <t>AMP</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>'0203020C0AAAAAA</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
-        </is>
-      </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>'21855511000001108</t>
+          <t>'10837011000001103</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (Focus Pharmaceuticals Ltd)</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Adenosine 6mg/2ml solution for injection (Focus Pharmaceuticals Ltd) 6 vials</t>
+          <t>Nutrison liquid (Waymade Healthcare Plc)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -751,24 +706,19 @@
           <t>AMP</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>'0203020C0AAAAAA</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
-        </is>
-      </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>'24530711000001102</t>
+          <t>'11160511000001103</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (Alliance Healthcare (Distribution) Ltd)</t>
+          <t>Nutrison liquid (Waymade Healthcare Plc)</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Nutrison (Waymade Healthcare Plc) 500 mls</t>
         </is>
       </c>
     </row>
@@ -783,36 +733,26 @@
           <t>AMP</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>'0203020C0AAAAAA</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
-        </is>
-      </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>'24531011000001108</t>
+          <t>'10837111000001102</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (Alliance Healthcare (Distribution) Ltd)</t>
+          <t>Nutrison liquid (Waymade Healthcare Plc)</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection (Alliance Healthcare (Distribution) Ltd) 6 vials</t>
+          <t>Nutrison (Waymade Healthcare Plc) 1000 mls</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -820,24 +760,19 @@
           <t>AMP</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>'0203020C0AAAAAA</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
-        </is>
-      </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>'34516211000001103</t>
+          <t>'15973011000001107</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (Peckforton Pharmaceuticals Ltd)</t>
+          <t>Nutrison liquid (Waymade Healthcare Plc)</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Nutrison (Waymade Healthcare Plc) 1500 mls</t>
         </is>
       </c>
     </row>
@@ -849,7 +784,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>AMP</t>
+          <t>VMP</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -864,24 +799,24 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>'34516411000001104</t>
+          <t>'4744111000001109</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection vials (Peckforton Pharmaceuticals Ltd)</t>
+          <t>Adenosine 6mg/2ml solution for injection vials</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Adenosine 6mg/2ml solution for injection (Peckforton Pharmaceuticals Ltd) 5 vials</t>
+          <t>Adenosine 6mg/2ml solution for injection 6 vials</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -891,59 +826,59 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>'1003020U0AAAIAI</t>
+          <t>'0203020C0AAAAAA</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Diclofenac Sod_Gel 2.32%</t>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>'22480211000001104</t>
+          <t>'34516311000001106</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% gel</t>
+          <t>Adenosine 6mg/2ml solution for injection vials</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection 5 vials</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMP</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>'1003020U0AAAIAI</t>
+          <t>'0203020C0BBAAAA</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Diclofenac Sod_Gel 2.32%</t>
+          <t>Adenocor_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>'22479411000001100</t>
+          <t>'4744411000001104</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% gel</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Diclofenac 2.32% 50 grams</t>
+          <t>Adenocor 6mg/2ml solution for injection vials (Sanofi)</t>
         </is>
       </c>
     </row>
@@ -955,76 +890,71 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMP</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>'1003020U0AAAIAI</t>
+          <t>'0203020C0BBAAAA</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Diclofenac Sod_Gel 2.32%</t>
+          <t>Adenocor_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>'22479511000001101</t>
+          <t>'4744711000001105</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% gel</t>
+          <t>Adenocor 6mg/2ml solution for injection vials (Sanofi)</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% 30 grams</t>
+          <t>Adenocor 6mg/2ml solution for injection (Sanofi) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>VMP</t>
+          <t>AMP</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>'1003020U0AAAIAI</t>
+          <t>'0203020C0AAAAAA</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Diclofenac Sod_Gel 2.32%</t>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>'26352411000001101</t>
+          <t>'19663311000001109</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Diclofenac 2.32% gel</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Diclofenac 2.32% 100 grams</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Wockhardt UK Ltd)</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Presentation</t>
+          <t>Pack</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1034,29 +964,34 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>'1003020U0BBADAI</t>
+          <t>'0203020C0AAAAAA</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>'22479611000001102</t>
+          <t>'19663411000001102</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (Wockhardt UK Ltd)</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection (Wockhardt UK Ltd) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1066,27 +1001,22 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>'1003020U0BBADAI</t>
+          <t>'0203020C0AAAAAA</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>'22479711000001106</t>
+          <t>'20009311000001102</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 50 grams</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (A A H Pharmaceuticals Ltd)</t>
         </is>
       </c>
     </row>
@@ -1103,34 +1033,34 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>'1003020U0BBADAI</t>
+          <t>'0203020C0AAAAAA</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>'22479911000001108</t>
+          <t>'20009411000001109</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+          <t>Adenosine 6mg/2ml solution for injection vials (A A H Pharmaceuticals Ltd)</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 30 grams</t>
+          <t>Adenosine 6mg/2ml solution for injection (A A H Pharmaceuticals Ltd) 6 vials</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Pack</t>
+          <t>Presentation</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1140,27 +1070,1151 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>'0203020C0AAAAAA</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>'21855411000001109</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection vials (Focus Pharmaceuticals Ltd)</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>'0203020C0AAAAAA</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>'21855511000001108</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection vials (Focus Pharmaceuticals Ltd)</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection (Focus Pharmaceuticals Ltd) 6 vials</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>'0203020C0AAAAAA</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>'24530711000001102</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection vials (Alliance Healthcare (Distribution) Ltd)</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>'0203020C0AAAAAA</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>'24531011000001108</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection vials (Alliance Healthcare (Distribution) Ltd)</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection (Alliance Healthcare (Distribution) Ltd) 6 vials</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>'0203020C0AAAAAA</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>'34516211000001103</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection vials (Peckforton Pharmaceuticals Ltd)</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>'0203020C0AAAAAA</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Adenosine_I/V Inf 3mg/ml 2ml Vl</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>'34516411000001104</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection vials (Peckforton Pharmaceuticals Ltd)</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Adenosine 6mg/2ml solution for injection (Peckforton Pharmaceuticals Ltd) 5 vials</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>'1106000X0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Piloc HCl_Eye Dps 6%</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>'9393611000001106</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative free</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative 1 ml</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>'1106000X0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Piloc HCl_Eye Dps 6%</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>'20293311000001106</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative free</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative 10 mls</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>'1106000X0AAA4A4</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Piloc HCl_Eye Dps 6% P/F</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>'9393711000001102</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative free (Special Order)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>'1106000X0AAA4A4</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Piloc HCl_Eye Dps 6% P/F</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>'9393811000001105</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative free (Special Order)</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative (Special Order) 1 ml</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>'1106000X0AAA4A4</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Piloc HCl_Eye Dps 6% P/F</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>'20293411000001104</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative free (Special Order)</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops preservative (Special Order) 10 mls</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>'1106000X0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Piloc HCl_Eye Dps 6%</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>'347208002</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>'1106000X0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Piloc HCl_Eye Dps 6%</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>'9394111000001101</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye 1 ml</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>'1106000X0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Piloc HCl_Eye Dps 6%</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>'20293111000001109</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye 10 mls</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>'1106000X0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Piloc HCl_Eye Dps 6%</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>'9394311000001104</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops (Special Order)</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>'1106000X0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Piloc HCl_Eye Dps 6%</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>'9394411000001106</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops (Special Order)</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye (Special Order) 1 ml</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>'1106000X0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Piloc HCl_Eye Dps 6%</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>'20293211000001103</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye drops (Special Order)</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Pilocarpine hydrochloride 6% eye (Special Order) 10 mls</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>'1003020U0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Diclofenac Sod_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>'22480211000001104</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% gel</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>'1003020U0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Diclofenac Sod_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>'22479411000001100</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% gel</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% 50 grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>'1003020U0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Diclofenac Sod_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>'22479511000001101</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% gel</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% 30 grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>'1003020U0AAAIAI</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Diclofenac Sod_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>'26352411000001101</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% gel</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Diclofenac 2.32% 100 grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
           <t>'1003020U0BBADAI</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>'22479611000001102</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>'1003020U0BBADAI</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>'22479711000001106</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 50 grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>'1003020U0BBADAI</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>'22479911000001108</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 30 grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>'1003020U0BBADAI</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Voltarol 12 Hour Emulgel P_Gel 2.32%</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
         <is>
           <t>'26352611000001103</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F47" t="inlineStr">
         <is>
           <t>Voltarol 12 Hour Emulgel P 2.32% gel (GlaxoSmithKline Consumer Healthcare)</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="G47" t="inlineStr">
         <is>
           <t>Voltarol 12 Hour Emulgel P 2.32% (GlaxoSmithKline Consumer Healthcare) 100 grams</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>'1305020C0AAFVFV</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Coal Tar 10%/Salic Acid 5%/Aq_Crm</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>'28789311000001103</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous cream</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>'1305020C0AAFVFV</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Coal Tar 10%/Salic Acid 5%/Aq_Crm</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>'28781611000001107</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous cream</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous 1 gram</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>'1305020C0AAFVFV</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Coal Tar 10%/Salic Acid 5%/Aq_Crm</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>'28781711000001103</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous cream (Special Order)</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>'1305020C0AAFVFV</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Coal Tar 10%/Salic Acid 5%/Aq_Crm</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>'28781811000001106</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous cream (Special Order)</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>Coal tar solution 10% / Salicylic acid 5% in Aqueous (Special Order) 1 gram</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>'1305020C0AAFVFV</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Coal Tar 10%/Salic Acid 5%/Aq_Crm</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>'28946311000001106</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Coal tar 10% / Salicylic acid 5% in Aqueous cream</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>VMP</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>'1305020C0AAFVFV</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Coal Tar 10%/Salic Acid 5%/Aq_Crm</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>'28942411000001100</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Coal tar 10% / Salicylic acid 5% in Aqueous cream</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Coal tar 10% / Salicylic acid 5% in Aqueous 1 gram</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Presentation</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>'1305020C0AAFVFV</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Coal Tar 10%/Salic Acid 5%/Aq_Crm</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>'28942511000001101</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Coal tar 10% / Salicylic acid 5% in Aqueous cream (Special Order)</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Pack</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>AMP</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>'1305020C0AAFVFV</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Coal Tar 10%/Salic Acid 5%/Aq_Crm</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>'28942611000001102</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Coal tar 10% / Salicylic acid 5% in Aqueous cream (Special Order)</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>Coal tar 10% / Salicylic acid 5% in Aqueous (Special Order) 1 gram</t>
         </is>
       </c>
     </row>

</xml_diff>